<commit_message>
graph update for 1a
</commit_message>
<xml_diff>
--- a/exp1a/output.xlsx
+++ b/exp1a/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen03/Dev/repos/stepDAA/exp1a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F501C17A-D2AD-1847-905B-4DB01B4E97E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80956A31-3C8F-F14B-8F34-EEEF3063934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1665,8 +1665,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2179,8 +2180,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3058,14 +3060,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3116,6 +3172,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>f(n)</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5386,7 +5501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="75" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>